<commit_message>
ajustement equipe et horaire suite au désistement de Vincent
</commit_message>
<xml_diff>
--- a/template/equipe.xlsx
+++ b/template/equipe.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/etiennerivard/notes_de_cours/techinfo/template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0218540-3FED-F347-AD0C-8E763AAF593C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF75DE2C-A4C9-5841-B45D-745DEE4F0F8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17620" xr2:uid="{6B795B45-6C14-B04F-B93D-A59A5BE3A68D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="50">
   <si>
     <t>nom</t>
   </si>
@@ -86,9 +86,6 @@
     <t>https://teams.microsoft.com/l/chat/0/0?tenantId=9d6cf526-ad81-46f8-a73a-a507aaf06cda&amp;users=OUELLET.ALEXANDRE@cegepvicto.ca</t>
   </si>
   <si>
-    <t>(819) 758-6401 poste 2520</t>
-  </si>
-  <si>
     <t>Carine Croteau</t>
   </si>
   <si>
@@ -173,12 +170,6 @@
     <t>/assets/frederik-taleb.jpeg</t>
   </si>
   <si>
-    <t>Vincent Chrétien</t>
-  </si>
-  <si>
-    <t>chretien.vincent@cegepvicto.ca</t>
-  </si>
-  <si>
     <t>chaieb.cirine@cegepvicto.ca</t>
   </si>
   <si>
@@ -188,7 +179,13 @@
     <t>https://teams.microsoft.com/l/chat/0/0?tenantId=9d6cf526-ad81-46f8-a73a-a507aaf06cda&amp;users=CHAIEB.CIRINE@cegepvicto.ca</t>
   </si>
   <si>
-    <t>https://teams.microsoft.com/l/chat/0/0?tenantId=9d6cf526-ad81-46f8-a73a-a507aaf06cda&amp;users=CHRETIEN.VINCENT@cegepvicto.ca</t>
+    <t>Sébastien Trottier</t>
+  </si>
+  <si>
+    <t>trottier.sebastien@cegepvicto.ca</t>
+  </si>
+  <si>
+    <t>https://teams.microsoft.com/l/chat/0/0?tenantId=9d6cf526-ad81-46f8-a73a-a507aaf06cda&amp;users=TROTTIER.SEBASTIEN@cegepvicto.ca</t>
   </si>
 </sst>
 </file>
@@ -585,7 +582,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -625,7 +622,7 @@
         <v>13</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>14</v>
@@ -642,56 +639,56 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="4" t="s">
         <v>18</v>
-      </c>
-      <c r="E3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D4" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="4" t="s">
         <v>25</v>
-      </c>
-      <c r="E4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E5" t="s">
         <v>9</v>
@@ -700,7 +697,7 @@
         <v>10</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -708,7 +705,7 @@
         <v>7</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>8</v>
@@ -725,79 +722,79 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D7" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" s="4" t="s">
         <v>28</v>
-      </c>
-      <c r="E7" t="s">
-        <v>9</v>
-      </c>
-      <c r="F7" t="s">
-        <v>10</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D8" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" s="4" t="s">
         <v>31</v>
-      </c>
-      <c r="E8" t="s">
-        <v>9</v>
-      </c>
-      <c r="F8" t="s">
-        <v>10</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="C9" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D9" s="3" t="s">
+      <c r="E9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9" s="4" t="s">
         <v>22</v>
-      </c>
-      <c r="E9" t="s">
-        <v>9</v>
-      </c>
-      <c r="F9" t="s">
-        <v>10</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>33</v>
+        <v>47</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="E10" t="s">
         <v>9</v>
@@ -806,33 +803,33 @@
         <v>10</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>35</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="B11" s="1"/>
-      <c r="C11" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>46</v>
+      <c r="C11" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>33</v>
       </c>
       <c r="E11" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="F11" t="s">
         <v>10</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>50</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G11">
-    <sortCondition ref="A2:A11"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G10">
+    <sortCondition ref="A2:A10"/>
   </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
@@ -850,15 +847,15 @@
     <hyperlink ref="G7" r:id="rId12" xr:uid="{263A76BA-B256-4A29-B498-E208EBF8E687}"/>
     <hyperlink ref="D8" r:id="rId13" xr:uid="{8800F2D9-30C8-4D1C-9E71-40C42A1B9FC3}"/>
     <hyperlink ref="G8" r:id="rId14" xr:uid="{90E6A9A5-6765-442D-8285-2B88419E6497}"/>
-    <hyperlink ref="D10" r:id="rId15" xr:uid="{82F16C65-70BD-4E57-9878-8DDF0271C983}"/>
+    <hyperlink ref="D10" r:id="rId15" display="tousignant.simon@cegepvicto.ca" xr:uid="{82F16C65-70BD-4E57-9878-8DDF0271C983}"/>
     <hyperlink ref="G10" r:id="rId16" xr:uid="{F736E8AE-53A5-451A-8F20-1D7C3122FD6F}"/>
     <hyperlink ref="C10" r:id="rId17" xr:uid="{EA23CE95-4D78-4412-AA6C-BDC25B91A8B8}"/>
-    <hyperlink ref="C11" r:id="rId18" xr:uid="{DFAA18E3-73CE-4E8E-B150-33A34FCF3524}"/>
-    <hyperlink ref="C5" r:id="rId19" xr:uid="{E449A7D7-BE44-412F-AD3B-E8CAE14A8738}"/>
-    <hyperlink ref="D11" r:id="rId20" xr:uid="{F17F7A0D-5618-EC49-9074-5FCB170C86AA}"/>
-    <hyperlink ref="D5" r:id="rId21" xr:uid="{2CCFFA7B-3F9E-4144-8474-7F58DD0171D7}"/>
-    <hyperlink ref="G5" r:id="rId22" xr:uid="{A5939AC6-7AF0-0B4F-902A-2522BB67B6F0}"/>
-    <hyperlink ref="G11" r:id="rId23" xr:uid="{288D7EE7-F9D0-B740-A334-379522DFC772}"/>
+    <hyperlink ref="C5" r:id="rId18" xr:uid="{E449A7D7-BE44-412F-AD3B-E8CAE14A8738}"/>
+    <hyperlink ref="D5" r:id="rId19" xr:uid="{2CCFFA7B-3F9E-4144-8474-7F58DD0171D7}"/>
+    <hyperlink ref="G5" r:id="rId20" xr:uid="{A5939AC6-7AF0-0B4F-902A-2522BB67B6F0}"/>
+    <hyperlink ref="D11" r:id="rId21" xr:uid="{2DFF4878-77A7-3147-BB6A-6F99564224C2}"/>
+    <hyperlink ref="G11" r:id="rId22" xr:uid="{0342F727-AE7C-6640-AFBE-6581114A221F}"/>
+    <hyperlink ref="C11" r:id="rId23" xr:uid="{F3C9B75E-3DE9-B24C-AE26-1DB2B3BEBC66}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
ajout photos pour équipe
</commit_message>
<xml_diff>
--- a/template/equipe.xlsx
+++ b/template/equipe.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/etiennerivard/notes_de_cours/techinfo/template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF75DE2C-A4C9-5841-B45D-745DEE4F0F8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{125F9959-30A7-FF43-910F-AF6652659C6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17620" xr2:uid="{6B795B45-6C14-B04F-B93D-A59A5BE3A68D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="51">
   <si>
     <t>nom</t>
   </si>
@@ -143,12 +143,6 @@
     <t>https://teams.microsoft.com/l/chat/0/0?tenantId=9d6cf526-ad81-46f8-a73a-a507aaf06cda&amp;users=TOUSIGNANT.SIMON@cegepvicto.ca</t>
   </si>
   <si>
-    <t>https://avatar.iran.liara.run/public/boy</t>
-  </si>
-  <si>
-    <t>https://avatar.iran.liara.run/public/girl</t>
-  </si>
-  <si>
     <t>/assets/etienne-rivard.png</t>
   </si>
   <si>
@@ -186,6 +180,15 @@
   </si>
   <si>
     <t>https://teams.microsoft.com/l/chat/0/0?tenantId=9d6cf526-ad81-46f8-a73a-a507aaf06cda&amp;users=TROTTIER.SEBASTIEN@cegepvicto.ca</t>
+  </si>
+  <si>
+    <t>/assets/sebastien_trottier.jpg</t>
+  </si>
+  <si>
+    <t>/assets/cirine-chaieb.png</t>
+  </si>
+  <si>
+    <t>/assets/placeholder-man.webp</t>
   </si>
 </sst>
 </file>
@@ -236,14 +239,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -582,12 +584,12 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="32.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="36" customWidth="1"/>
   </cols>
   <sheetData>
@@ -622,7 +624,7 @@
         <v>13</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>14</v>
@@ -643,7 +645,7 @@
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>17</v>
@@ -664,7 +666,7 @@
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>24</v>
@@ -681,23 +683,23 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B5" s="1"/>
-      <c r="C5" s="6" t="s">
-        <v>36</v>
+      <c r="C5" s="1" t="s">
+        <v>49</v>
       </c>
       <c r="D5" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="4" t="s">
         <v>44</v>
-      </c>
-      <c r="E5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -705,7 +707,7 @@
         <v>7</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>8</v>
@@ -726,7 +728,7 @@
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>27</v>
@@ -747,7 +749,7 @@
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>30</v>
@@ -770,7 +772,7 @@
         <v>20</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>21</v>
@@ -787,23 +789,23 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>45</v>
+      </c>
+      <c r="B10" s="1"/>
+      <c r="C10" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10" t="s">
+        <v>10</v>
+      </c>
+      <c r="G10" s="4" t="s">
         <v>47</v>
-      </c>
-      <c r="B10" s="1"/>
-      <c r="C10" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="E10" t="s">
-        <v>9</v>
-      </c>
-      <c r="F10" t="s">
-        <v>10</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
@@ -812,7 +814,7 @@
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="4" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>33</v>
@@ -849,13 +851,11 @@
     <hyperlink ref="G8" r:id="rId14" xr:uid="{90E6A9A5-6765-442D-8285-2B88419E6497}"/>
     <hyperlink ref="D10" r:id="rId15" display="tousignant.simon@cegepvicto.ca" xr:uid="{82F16C65-70BD-4E57-9878-8DDF0271C983}"/>
     <hyperlink ref="G10" r:id="rId16" xr:uid="{F736E8AE-53A5-451A-8F20-1D7C3122FD6F}"/>
-    <hyperlink ref="C10" r:id="rId17" xr:uid="{EA23CE95-4D78-4412-AA6C-BDC25B91A8B8}"/>
-    <hyperlink ref="C5" r:id="rId18" xr:uid="{E449A7D7-BE44-412F-AD3B-E8CAE14A8738}"/>
-    <hyperlink ref="D5" r:id="rId19" xr:uid="{2CCFFA7B-3F9E-4144-8474-7F58DD0171D7}"/>
-    <hyperlink ref="G5" r:id="rId20" xr:uid="{A5939AC6-7AF0-0B4F-902A-2522BB67B6F0}"/>
-    <hyperlink ref="D11" r:id="rId21" xr:uid="{2DFF4878-77A7-3147-BB6A-6F99564224C2}"/>
-    <hyperlink ref="G11" r:id="rId22" xr:uid="{0342F727-AE7C-6640-AFBE-6581114A221F}"/>
-    <hyperlink ref="C11" r:id="rId23" xr:uid="{F3C9B75E-3DE9-B24C-AE26-1DB2B3BEBC66}"/>
+    <hyperlink ref="D5" r:id="rId17" xr:uid="{2CCFFA7B-3F9E-4144-8474-7F58DD0171D7}"/>
+    <hyperlink ref="G5" r:id="rId18" xr:uid="{A5939AC6-7AF0-0B4F-902A-2522BB67B6F0}"/>
+    <hyperlink ref="D11" r:id="rId19" xr:uid="{2DFF4878-77A7-3147-BB6A-6F99564224C2}"/>
+    <hyperlink ref="G11" r:id="rId20" xr:uid="{0342F727-AE7C-6640-AFBE-6581114A221F}"/>
+    <hyperlink ref="C11" r:id="rId21" display="https://avatar.iran.liara.run/public/boy" xr:uid="{F3C9B75E-3DE9-B24C-AE26-1DB2B3BEBC66}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
changement horaire et responsabilites
</commit_message>
<xml_diff>
--- a/template/equipe.xlsx
+++ b/template/equipe.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/etiennerivard/notes_de_cours/techinfo/template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{125F9959-30A7-FF43-910F-AF6652659C6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA93A27C-553B-7D4D-8129-D42046D0DF26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17620" xr2:uid="{6B795B45-6C14-B04F-B93D-A59A5BE3A68D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="54">
   <si>
     <t>nom</t>
   </si>
@@ -189,6 +189,15 @@
   </si>
   <si>
     <t>/assets/placeholder-man.webp</t>
+  </si>
+  <si>
+    <t>Gabriel Montplaisir</t>
+  </si>
+  <si>
+    <t>montplaisir.gabriel@cegepvicto.ca</t>
+  </si>
+  <si>
+    <t>https://teams.microsoft.com/l/chat/0/0?tenantId=9d6cf526-ad81-46f8-a73a-a507aaf06cda&amp;users=MONTPLAISIR.GABRIEL@cegepvicto.ca</t>
   </si>
 </sst>
 </file>
@@ -581,10 +590,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46DF1DC5-63E0-A14F-8B6A-86AB73F394B2}">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -766,16 +775,14 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>19</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>21</v>
+        <v>51</v>
+      </c>
+      <c r="B9" s="1"/>
+      <c r="C9" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>52</v>
       </c>
       <c r="E9" t="s">
         <v>9</v>
@@ -784,19 +791,21 @@
         <v>10</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>22</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>45</v>
-      </c>
-      <c r="B10" s="1"/>
+        <v>19</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="C10" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>46</v>
+        <v>38</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>21</v>
       </c>
       <c r="E10" t="s">
         <v>9</v>
@@ -805,33 +814,54 @@
         <v>10</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>47</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>45</v>
+      </c>
+      <c r="B11" s="1"/>
+      <c r="C11" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E11" t="s">
+        <v>9</v>
+      </c>
+      <c r="F11" t="s">
+        <v>10</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>32</v>
       </c>
-      <c r="B11" s="1"/>
-      <c r="C11" s="4" t="s">
+      <c r="B12" s="1"/>
+      <c r="C12" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D12" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="E11" t="s">
-        <v>9</v>
-      </c>
-      <c r="F11" t="s">
-        <v>10</v>
-      </c>
-      <c r="G11" s="4" t="s">
+      <c r="E12" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" t="s">
+        <v>10</v>
+      </c>
+      <c r="G12" s="4" t="s">
         <v>34</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G10">
-    <sortCondition ref="A2:A10"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G11">
+    <sortCondition ref="A2:A11"/>
   </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
@@ -841,21 +871,24 @@
     <hyperlink ref="G2" r:id="rId4" xr:uid="{F550D781-4855-4E10-88FA-3A222809FFB7}"/>
     <hyperlink ref="D3" r:id="rId5" xr:uid="{9443F340-71D8-40D6-A0C9-35D0D38C5BC2}"/>
     <hyperlink ref="G3" r:id="rId6" xr:uid="{1B226E6A-263C-43AE-9CCA-EC842F5E59CA}"/>
-    <hyperlink ref="D9" r:id="rId7" xr:uid="{4C97C5B1-71FC-4BB8-8E2C-430E1A58D443}"/>
-    <hyperlink ref="G9" r:id="rId8" xr:uid="{F77BBB30-0E91-4834-992D-8C3E6F3FF743}"/>
+    <hyperlink ref="D10" r:id="rId7" xr:uid="{4C97C5B1-71FC-4BB8-8E2C-430E1A58D443}"/>
+    <hyperlink ref="G10" r:id="rId8" xr:uid="{F77BBB30-0E91-4834-992D-8C3E6F3FF743}"/>
     <hyperlink ref="D4" r:id="rId9" xr:uid="{44F3169D-D34E-464F-A7BB-69732F62CD5B}"/>
     <hyperlink ref="G4" r:id="rId10" xr:uid="{F739B185-8900-4D37-A986-42B107B5BD3B}"/>
     <hyperlink ref="D7" r:id="rId11" xr:uid="{70C39852-F2CE-4E7F-AB0A-5CA460ECC68C}"/>
     <hyperlink ref="G7" r:id="rId12" xr:uid="{263A76BA-B256-4A29-B498-E208EBF8E687}"/>
     <hyperlink ref="D8" r:id="rId13" xr:uid="{8800F2D9-30C8-4D1C-9E71-40C42A1B9FC3}"/>
     <hyperlink ref="G8" r:id="rId14" xr:uid="{90E6A9A5-6765-442D-8285-2B88419E6497}"/>
-    <hyperlink ref="D10" r:id="rId15" display="tousignant.simon@cegepvicto.ca" xr:uid="{82F16C65-70BD-4E57-9878-8DDF0271C983}"/>
-    <hyperlink ref="G10" r:id="rId16" xr:uid="{F736E8AE-53A5-451A-8F20-1D7C3122FD6F}"/>
+    <hyperlink ref="D11" r:id="rId15" display="tousignant.simon@cegepvicto.ca" xr:uid="{82F16C65-70BD-4E57-9878-8DDF0271C983}"/>
+    <hyperlink ref="G11" r:id="rId16" xr:uid="{F736E8AE-53A5-451A-8F20-1D7C3122FD6F}"/>
     <hyperlink ref="D5" r:id="rId17" xr:uid="{2CCFFA7B-3F9E-4144-8474-7F58DD0171D7}"/>
     <hyperlink ref="G5" r:id="rId18" xr:uid="{A5939AC6-7AF0-0B4F-902A-2522BB67B6F0}"/>
-    <hyperlink ref="D11" r:id="rId19" xr:uid="{2DFF4878-77A7-3147-BB6A-6F99564224C2}"/>
-    <hyperlink ref="G11" r:id="rId20" xr:uid="{0342F727-AE7C-6640-AFBE-6581114A221F}"/>
-    <hyperlink ref="C11" r:id="rId21" display="https://avatar.iran.liara.run/public/boy" xr:uid="{F3C9B75E-3DE9-B24C-AE26-1DB2B3BEBC66}"/>
+    <hyperlink ref="D12" r:id="rId19" xr:uid="{2DFF4878-77A7-3147-BB6A-6F99564224C2}"/>
+    <hyperlink ref="G12" r:id="rId20" xr:uid="{0342F727-AE7C-6640-AFBE-6581114A221F}"/>
+    <hyperlink ref="C12" r:id="rId21" display="https://avatar.iran.liara.run/public/boy" xr:uid="{F3C9B75E-3DE9-B24C-AE26-1DB2B3BEBC66}"/>
+    <hyperlink ref="D9" r:id="rId22" display="tousignant.simon@cegepvicto.ca" xr:uid="{D913369C-A340-9E43-B8C0-2AFCAB28EEC2}"/>
+    <hyperlink ref="G9" r:id="rId23" xr:uid="{2419F377-2062-014F-94C7-474FF811CBB1}"/>
+    <hyperlink ref="C9" r:id="rId24" display="https://avatar.iran.liara.run/public/boy" xr:uid="{BCD8AE23-3919-FC48-8463-CF5B4BB73571}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
changement horaire + niveaux IA
</commit_message>
<xml_diff>
--- a/template/equipe.xlsx
+++ b/template/equipe.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/etiennerivard/notes_de_cours/techinfo/template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA93A27C-553B-7D4D-8129-D42046D0DF26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A8BEA26-1CE4-8743-B63E-5F4143CDFBC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17620" xr2:uid="{6B795B45-6C14-B04F-B93D-A59A5BE3A68D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="39">
   <si>
     <t>nom</t>
   </si>
@@ -86,15 +86,6 @@
     <t>https://teams.microsoft.com/l/chat/0/0?tenantId=9d6cf526-ad81-46f8-a73a-a507aaf06cda&amp;users=OUELLET.ALEXANDRE@cegepvicto.ca</t>
   </si>
   <si>
-    <t>Carine Croteau</t>
-  </si>
-  <si>
-    <t>croteau.carine@cegepvicto.ca</t>
-  </si>
-  <si>
-    <t>https://teams.microsoft.com/l/chat/0/0?tenantId=9d6cf526-ad81-46f8-a73a-a507aaf06cda&amp;users=CROTEAU.CARINE@cegepvicto.ca</t>
-  </si>
-  <si>
     <t>Mathieu Fréchette</t>
   </si>
   <si>
@@ -149,9 +140,6 @@
     <t>/assets/alexandre-ouellet.png</t>
   </si>
   <si>
-    <t>/assets/carine-croteau.jpeg</t>
-  </si>
-  <si>
     <t>/assets/mathieu-frechette.jpeg</t>
   </si>
   <si>
@@ -164,40 +152,7 @@
     <t>/assets/frederik-taleb.jpeg</t>
   </si>
   <si>
-    <t>chaieb.cirine@cegepvicto.ca</t>
-  </si>
-  <si>
-    <t>Cirine Chaieb</t>
-  </si>
-  <si>
-    <t>https://teams.microsoft.com/l/chat/0/0?tenantId=9d6cf526-ad81-46f8-a73a-a507aaf06cda&amp;users=CHAIEB.CIRINE@cegepvicto.ca</t>
-  </si>
-  <si>
-    <t>Sébastien Trottier</t>
-  </si>
-  <si>
-    <t>trottier.sebastien@cegepvicto.ca</t>
-  </si>
-  <si>
-    <t>https://teams.microsoft.com/l/chat/0/0?tenantId=9d6cf526-ad81-46f8-a73a-a507aaf06cda&amp;users=TROTTIER.SEBASTIEN@cegepvicto.ca</t>
-  </si>
-  <si>
-    <t>/assets/sebastien_trottier.jpg</t>
-  </si>
-  <si>
-    <t>/assets/cirine-chaieb.png</t>
-  </si>
-  <si>
     <t>/assets/placeholder-man.webp</t>
-  </si>
-  <si>
-    <t>Gabriel Montplaisir</t>
-  </si>
-  <si>
-    <t>montplaisir.gabriel@cegepvicto.ca</t>
-  </si>
-  <si>
-    <t>https://teams.microsoft.com/l/chat/0/0?tenantId=9d6cf526-ad81-46f8-a73a-a507aaf06cda&amp;users=MONTPLAISIR.GABRIEL@cegepvicto.ca</t>
   </si>
 </sst>
 </file>
@@ -590,10 +545,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46DF1DC5-63E0-A14F-8B6A-86AB73F394B2}">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -633,7 +588,7 @@
         <v>13</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>14</v>
@@ -650,14 +605,14 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="E3" t="s">
         <v>9</v>
@@ -666,19 +621,18 @@
         <v>10</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="2" t="s">
-        <v>39</v>
+        <v>7</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="E4" t="s">
         <v>9</v>
@@ -687,19 +641,19 @@
         <v>10</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>43</v>
+        <v>23</v>
       </c>
       <c r="B5" s="1"/>
-      <c r="C5" s="1" t="s">
-        <v>49</v>
+      <c r="C5" s="2" t="s">
+        <v>36</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="E5" t="s">
         <v>9</v>
@@ -708,18 +662,19 @@
         <v>10</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>44</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>35</v>
+        <v>26</v>
+      </c>
+      <c r="B6" s="1"/>
+      <c r="C6" s="2" t="s">
+        <v>37</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="E6" t="s">
         <v>9</v>
@@ -728,19 +683,21 @@
         <v>10</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>26</v>
-      </c>
-      <c r="B7" s="1"/>
+        <v>16</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="C7" s="2" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="E7" t="s">
         <v>9</v>
@@ -749,7 +706,7 @@
         <v>10</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -757,10 +714,10 @@
         <v>29</v>
       </c>
       <c r="B8" s="1"/>
-      <c r="C8" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D8" s="3" t="s">
+      <c r="C8" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" s="5" t="s">
         <v>30</v>
       </c>
       <c r="E8" t="s">
@@ -773,122 +730,27 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>51</v>
-      </c>
-      <c r="B9" s="1"/>
-      <c r="C9" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="E9" t="s">
-        <v>9</v>
-      </c>
-      <c r="F9" t="s">
-        <v>10</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>19</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E10" t="s">
-        <v>9</v>
-      </c>
-      <c r="F10" t="s">
-        <v>10</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>45</v>
-      </c>
-      <c r="B11" s="1"/>
-      <c r="C11" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="E11" t="s">
-        <v>9</v>
-      </c>
-      <c r="F11" t="s">
-        <v>10</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>32</v>
-      </c>
-      <c r="B12" s="1"/>
-      <c r="C12" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="E12" t="s">
-        <v>9</v>
-      </c>
-      <c r="F12" t="s">
-        <v>10</v>
-      </c>
-      <c r="G12" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G11">
-    <sortCondition ref="A2:A11"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G7">
+    <sortCondition ref="A2:A7"/>
   </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="D6" r:id="rId1" xr:uid="{F789545C-CEF6-4B3A-9358-1A6F9E968CF2}"/>
-    <hyperlink ref="G6" r:id="rId2" xr:uid="{142F557C-F7AB-411D-B17A-5FCFF3CE21F9}"/>
+    <hyperlink ref="D4" r:id="rId1" xr:uid="{F789545C-CEF6-4B3A-9358-1A6F9E968CF2}"/>
+    <hyperlink ref="G4" r:id="rId2" xr:uid="{142F557C-F7AB-411D-B17A-5FCFF3CE21F9}"/>
     <hyperlink ref="D2" r:id="rId3" xr:uid="{47C36387-4B68-48E7-B056-2081D1996CF5}"/>
     <hyperlink ref="G2" r:id="rId4" xr:uid="{F550D781-4855-4E10-88FA-3A222809FFB7}"/>
-    <hyperlink ref="D3" r:id="rId5" xr:uid="{9443F340-71D8-40D6-A0C9-35D0D38C5BC2}"/>
-    <hyperlink ref="G3" r:id="rId6" xr:uid="{1B226E6A-263C-43AE-9CCA-EC842F5E59CA}"/>
-    <hyperlink ref="D10" r:id="rId7" xr:uid="{4C97C5B1-71FC-4BB8-8E2C-430E1A58D443}"/>
-    <hyperlink ref="G10" r:id="rId8" xr:uid="{F77BBB30-0E91-4834-992D-8C3E6F3FF743}"/>
-    <hyperlink ref="D4" r:id="rId9" xr:uid="{44F3169D-D34E-464F-A7BB-69732F62CD5B}"/>
-    <hyperlink ref="G4" r:id="rId10" xr:uid="{F739B185-8900-4D37-A986-42B107B5BD3B}"/>
-    <hyperlink ref="D7" r:id="rId11" xr:uid="{70C39852-F2CE-4E7F-AB0A-5CA460ECC68C}"/>
-    <hyperlink ref="G7" r:id="rId12" xr:uid="{263A76BA-B256-4A29-B498-E208EBF8E687}"/>
-    <hyperlink ref="D8" r:id="rId13" xr:uid="{8800F2D9-30C8-4D1C-9E71-40C42A1B9FC3}"/>
-    <hyperlink ref="G8" r:id="rId14" xr:uid="{90E6A9A5-6765-442D-8285-2B88419E6497}"/>
-    <hyperlink ref="D11" r:id="rId15" display="tousignant.simon@cegepvicto.ca" xr:uid="{82F16C65-70BD-4E57-9878-8DDF0271C983}"/>
-    <hyperlink ref="G11" r:id="rId16" xr:uid="{F736E8AE-53A5-451A-8F20-1D7C3122FD6F}"/>
-    <hyperlink ref="D5" r:id="rId17" xr:uid="{2CCFFA7B-3F9E-4144-8474-7F58DD0171D7}"/>
-    <hyperlink ref="G5" r:id="rId18" xr:uid="{A5939AC6-7AF0-0B4F-902A-2522BB67B6F0}"/>
-    <hyperlink ref="D12" r:id="rId19" xr:uid="{2DFF4878-77A7-3147-BB6A-6F99564224C2}"/>
-    <hyperlink ref="G12" r:id="rId20" xr:uid="{0342F727-AE7C-6640-AFBE-6581114A221F}"/>
-    <hyperlink ref="C12" r:id="rId21" display="https://avatar.iran.liara.run/public/boy" xr:uid="{F3C9B75E-3DE9-B24C-AE26-1DB2B3BEBC66}"/>
-    <hyperlink ref="D9" r:id="rId22" display="tousignant.simon@cegepvicto.ca" xr:uid="{D913369C-A340-9E43-B8C0-2AFCAB28EEC2}"/>
-    <hyperlink ref="G9" r:id="rId23" xr:uid="{2419F377-2062-014F-94C7-474FF811CBB1}"/>
-    <hyperlink ref="C9" r:id="rId24" display="https://avatar.iran.liara.run/public/boy" xr:uid="{BCD8AE23-3919-FC48-8463-CF5B4BB73571}"/>
+    <hyperlink ref="D7" r:id="rId5" xr:uid="{4C97C5B1-71FC-4BB8-8E2C-430E1A58D443}"/>
+    <hyperlink ref="G7" r:id="rId6" xr:uid="{F77BBB30-0E91-4834-992D-8C3E6F3FF743}"/>
+    <hyperlink ref="D3" r:id="rId7" xr:uid="{44F3169D-D34E-464F-A7BB-69732F62CD5B}"/>
+    <hyperlink ref="G3" r:id="rId8" xr:uid="{F739B185-8900-4D37-A986-42B107B5BD3B}"/>
+    <hyperlink ref="D5" r:id="rId9" xr:uid="{70C39852-F2CE-4E7F-AB0A-5CA460ECC68C}"/>
+    <hyperlink ref="G5" r:id="rId10" xr:uid="{263A76BA-B256-4A29-B498-E208EBF8E687}"/>
+    <hyperlink ref="D6" r:id="rId11" xr:uid="{8800F2D9-30C8-4D1C-9E71-40C42A1B9FC3}"/>
+    <hyperlink ref="G6" r:id="rId12" xr:uid="{90E6A9A5-6765-442D-8285-2B88419E6497}"/>
+    <hyperlink ref="D8" r:id="rId13" xr:uid="{2DFF4878-77A7-3147-BB6A-6F99564224C2}"/>
+    <hyperlink ref="G8" r:id="rId14" xr:uid="{0342F727-AE7C-6640-AFBE-6581114A221F}"/>
+    <hyperlink ref="C8" r:id="rId15" display="https://avatar.iran.liara.run/public/boy" xr:uid="{F3C9B75E-3DE9-B24C-AE26-1DB2B3BEBC66}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
nouvelle photo François + sites de cours
</commit_message>
<xml_diff>
--- a/template/equipe.xlsx
+++ b/template/equipe.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10727"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/etiennerivard/notes_de_cours/techinfo/template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A8BEA26-1CE4-8743-B63E-5F4143CDFBC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B77657A-0850-3F4C-A0F6-735295A31A32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17620" xr2:uid="{6B795B45-6C14-B04F-B93D-A59A5BE3A68D}"/>
   </bookViews>
@@ -146,13 +146,13 @@
     <t>/assets/christiane-lagace.jpeg</t>
   </si>
   <si>
-    <t>/assets/francois-mercier.jpeg</t>
-  </si>
-  <si>
     <t>/assets/frederik-taleb.jpeg</t>
   </si>
   <si>
     <t>/assets/placeholder-man.webp</t>
+  </si>
+  <si>
+    <t>/assets/francois-mercier.png</t>
   </si>
 </sst>
 </file>
@@ -548,7 +548,7 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -650,7 +650,7 @@
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>24</v>
@@ -671,7 +671,7 @@
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>27</v>
@@ -715,7 +715,7 @@
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>30</v>

</xml_diff>